<commit_message>
feat: study, building, space, instrument models and forms updated
</commit_message>
<xml_diff>
--- a/backend/api/data/Dictionary_data.xlsx
+++ b/backend/api/data/Dictionary_data.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://epflch.sharepoint.com/sites/ENAC-IT/Documents partages/Research IT/Advanced Services/0002 – PILOT iAQ/Pilot_iAQ_Shared/Data/Metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{67B11E78-C067-4E63-B1B5-7B4C3D8D465D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="76" documentId="13_ncr:1_{B4387AF4-D70C-3F4F-B95E-A761DDA3FAD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BDA0B682-3EFD-8A43-A10B-054DC270C147}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="29400" windowHeight="16840" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16640" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Individual VOC" sheetId="1" r:id="rId1"/>
     <sheet name="Time series" sheetId="2" r:id="rId2"/>
     <sheet name="Other parameter" sheetId="3" r:id="rId3"/>
     <sheet name="Bio contaminant" sheetId="4" r:id="rId4"/>
+    <sheet name="For filter selection" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="669">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1589" uniqueCount="675">
   <si>
     <t>CAS Number</t>
   </si>
@@ -1934,9 +1935,6 @@
     <t>Particle number ≤1μm </t>
   </si>
   <si>
-    <t>Nanoparticles </t>
-  </si>
-  <si>
     <t>Carbon dioxide </t>
   </si>
   <si>
@@ -2046,13 +2044,34 @@
   </si>
   <si>
     <t>fungi</t>
+  </si>
+  <si>
+    <t>Column name - actual IAQ data</t>
+  </si>
+  <si>
+    <t>Nanoparticles number</t>
+  </si>
+  <si>
+    <t>Particle mass concentration</t>
+  </si>
+  <si>
+    <t>Individual VOC</t>
+  </si>
+  <si>
+    <t>Particle number concentration</t>
+  </si>
+  <si>
+    <t>Bio contaminant</t>
+  </si>
+  <si>
+    <t>Category - for filter selection</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2078,6 +2097,14 @@
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2115,7 +2142,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2136,6 +2163,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2441,17 +2469,17 @@
   <dimension ref="A1:K203"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" customWidth="1"/>
+    <col min="3" max="3" width="28.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2486,7 +2514,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2518,7 +2546,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -2544,7 +2572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -2570,7 +2598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -2596,7 +2624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -2622,7 +2650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -2648,7 +2676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -2674,7 +2702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -2700,7 +2728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -2726,7 +2754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -2752,7 +2780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -2778,7 +2806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -2804,7 +2832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -2830,7 +2858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>54</v>
       </c>
@@ -2856,7 +2884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>57</v>
       </c>
@@ -2882,7 +2910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>60</v>
       </c>
@@ -2908,7 +2936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>63</v>
       </c>
@@ -2934,7 +2962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>66</v>
       </c>
@@ -2960,7 +2988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>69</v>
       </c>
@@ -2986,7 +3014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>72</v>
       </c>
@@ -3012,7 +3040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>75</v>
       </c>
@@ -3038,7 +3066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>78</v>
       </c>
@@ -3064,7 +3092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>81</v>
       </c>
@@ -3090,7 +3118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>84</v>
       </c>
@@ -3116,7 +3144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>87</v>
       </c>
@@ -3142,7 +3170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>90</v>
       </c>
@@ -3168,7 +3196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>93</v>
       </c>
@@ -3194,7 +3222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>96</v>
       </c>
@@ -3220,7 +3248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>99</v>
       </c>
@@ -3246,7 +3274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>102</v>
       </c>
@@ -3272,7 +3300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>105</v>
       </c>
@@ -3298,7 +3326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>108</v>
       </c>
@@ -3324,7 +3352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>111</v>
       </c>
@@ -3350,7 +3378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>114</v>
       </c>
@@ -3376,7 +3404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>117</v>
       </c>
@@ -3402,7 +3430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>120</v>
       </c>
@@ -3428,7 +3456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>123</v>
       </c>
@@ -3454,7 +3482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>126</v>
       </c>
@@ -3480,7 +3508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>129</v>
       </c>
@@ -3506,7 +3534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>132</v>
       </c>
@@ -3532,7 +3560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>135</v>
       </c>
@@ -3558,7 +3586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>138</v>
       </c>
@@ -3584,7 +3612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>141</v>
       </c>
@@ -3610,7 +3638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>144</v>
       </c>
@@ -3636,7 +3664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>147</v>
       </c>
@@ -3662,7 +3690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>150</v>
       </c>
@@ -3688,7 +3716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>153</v>
       </c>
@@ -3714,7 +3742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>156</v>
       </c>
@@ -3740,7 +3768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>159</v>
       </c>
@@ -3766,7 +3794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>162</v>
       </c>
@@ -3792,7 +3820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>165</v>
       </c>
@@ -3818,7 +3846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>168</v>
       </c>
@@ -3844,7 +3872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>171</v>
       </c>
@@ -3870,7 +3898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>174</v>
       </c>
@@ -3896,7 +3924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>177</v>
       </c>
@@ -3922,7 +3950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>180</v>
       </c>
@@ -3948,7 +3976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>183</v>
       </c>
@@ -3974,7 +4002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>186</v>
       </c>
@@ -4000,7 +4028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>189</v>
       </c>
@@ -4026,7 +4054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>192</v>
       </c>
@@ -4052,7 +4080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>195</v>
       </c>
@@ -4078,7 +4106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>198</v>
       </c>
@@ -4104,7 +4132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>201</v>
       </c>
@@ -4130,7 +4158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>204</v>
       </c>
@@ -4156,7 +4184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>207</v>
       </c>
@@ -4182,7 +4210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>210</v>
       </c>
@@ -4208,7 +4236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>213</v>
       </c>
@@ -4234,7 +4262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>216</v>
       </c>
@@ -4260,7 +4288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>219</v>
       </c>
@@ -4286,7 +4314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>222</v>
       </c>
@@ -4312,7 +4340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>225</v>
       </c>
@@ -4338,7 +4366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>228</v>
       </c>
@@ -4364,7 +4392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>231</v>
       </c>
@@ -4390,7 +4418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>234</v>
       </c>
@@ -4416,7 +4444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>237</v>
       </c>
@@ -4442,7 +4470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>240</v>
       </c>
@@ -4468,7 +4496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>243</v>
       </c>
@@ -4494,7 +4522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>246</v>
       </c>
@@ -4520,7 +4548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>249</v>
       </c>
@@ -4546,7 +4574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>252</v>
       </c>
@@ -4572,7 +4600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>255</v>
       </c>
@@ -4598,7 +4626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>258</v>
       </c>
@@ -4624,7 +4652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>261</v>
       </c>
@@ -4650,7 +4678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>264</v>
       </c>
@@ -4676,7 +4704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>267</v>
       </c>
@@ -4702,7 +4730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>270</v>
       </c>
@@ -4728,7 +4756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>273</v>
       </c>
@@ -4754,7 +4782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>276</v>
       </c>
@@ -4780,7 +4808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>279</v>
       </c>
@@ -4806,7 +4834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>281</v>
       </c>
@@ -4832,7 +4860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>284</v>
       </c>
@@ -4858,7 +4886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>287</v>
       </c>
@@ -4884,7 +4912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>290</v>
       </c>
@@ -4910,7 +4938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>293</v>
       </c>
@@ -4936,7 +4964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>296</v>
       </c>
@@ -4962,7 +4990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>299</v>
       </c>
@@ -4988,7 +5016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>302</v>
       </c>
@@ -5014,7 +5042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>305</v>
       </c>
@@ -5040,7 +5068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>308</v>
       </c>
@@ -5066,7 +5094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:8">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>311</v>
       </c>
@@ -5092,7 +5120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:8">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>314</v>
       </c>
@@ -5118,7 +5146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:8">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>317</v>
       </c>
@@ -5144,7 +5172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:8">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>320</v>
       </c>
@@ -5170,7 +5198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:8">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>322</v>
       </c>
@@ -5196,7 +5224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:8">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>325</v>
       </c>
@@ -5222,7 +5250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:8">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>328</v>
       </c>
@@ -5248,7 +5276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:8">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>331</v>
       </c>
@@ -5274,7 +5302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:8">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>334</v>
       </c>
@@ -5300,7 +5328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:8">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>337</v>
       </c>
@@ -5326,7 +5354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:8">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>340</v>
       </c>
@@ -5352,7 +5380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:8">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>342</v>
       </c>
@@ -5378,7 +5406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:8">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>345</v>
       </c>
@@ -5404,7 +5432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:8">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>348</v>
       </c>
@@ -5430,7 +5458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:8">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>351</v>
       </c>
@@ -5456,7 +5484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:8">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>354</v>
       </c>
@@ -5482,7 +5510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:8">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>357</v>
       </c>
@@ -5508,7 +5536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:8">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>360</v>
       </c>
@@ -5534,7 +5562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:8">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>363</v>
       </c>
@@ -5560,7 +5588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:8">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>366</v>
       </c>
@@ -5586,7 +5614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:8">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>369</v>
       </c>
@@ -5612,7 +5640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:8">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>372</v>
       </c>
@@ -5638,7 +5666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:8">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>375</v>
       </c>
@@ -5664,7 +5692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:8">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>378</v>
       </c>
@@ -5690,7 +5718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:8">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>381</v>
       </c>
@@ -5716,7 +5744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:8">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>384</v>
       </c>
@@ -5742,7 +5770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:8">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>387</v>
       </c>
@@ -5768,7 +5796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:8">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>390</v>
       </c>
@@ -5794,7 +5822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:8">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>393</v>
       </c>
@@ -5820,7 +5848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:8">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>396</v>
       </c>
@@ -5846,7 +5874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:8">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>399</v>
       </c>
@@ -5872,7 +5900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:8">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>402</v>
       </c>
@@ -5898,7 +5926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:8">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>405</v>
       </c>
@@ -5924,7 +5952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:8">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>408</v>
       </c>
@@ -5950,7 +5978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:8">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>411</v>
       </c>
@@ -5976,7 +6004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:8">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>414</v>
       </c>
@@ -6002,7 +6030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:8">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>417</v>
       </c>
@@ -6028,7 +6056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:8">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>420</v>
       </c>
@@ -6054,7 +6082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:8">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>423</v>
       </c>
@@ -6080,7 +6108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:8">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>426</v>
       </c>
@@ -6106,7 +6134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:8">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>429</v>
       </c>
@@ -6132,7 +6160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:8">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>432</v>
       </c>
@@ -6158,7 +6186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:8">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>435</v>
       </c>
@@ -6184,7 +6212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:8">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>438</v>
       </c>
@@ -6210,7 +6238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:8">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>441</v>
       </c>
@@ -6236,7 +6264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:8">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>444</v>
       </c>
@@ -6262,7 +6290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:8">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>447</v>
       </c>
@@ -6288,7 +6316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:8">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>450</v>
       </c>
@@ -6314,7 +6342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:8">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>453</v>
       </c>
@@ -6340,7 +6368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:8">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>456</v>
       </c>
@@ -6366,7 +6394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:8">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>459</v>
       </c>
@@ -6392,7 +6420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:8">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>462</v>
       </c>
@@ -6418,7 +6446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:8">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>465</v>
       </c>
@@ -6444,7 +6472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:8">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>468</v>
       </c>
@@ -6470,7 +6498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:8">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>471</v>
       </c>
@@ -6496,7 +6524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:8">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>474</v>
       </c>
@@ -6522,7 +6550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:8">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>477</v>
       </c>
@@ -6548,7 +6576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:8">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>480</v>
       </c>
@@ -6574,7 +6602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:8">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>483</v>
       </c>
@@ -6600,7 +6628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:8">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>486</v>
       </c>
@@ -6626,7 +6654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:8">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>489</v>
       </c>
@@ -6652,7 +6680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:8">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>492</v>
       </c>
@@ -6678,7 +6706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:8">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>495</v>
       </c>
@@ -6704,7 +6732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:8">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>498</v>
       </c>
@@ -6730,7 +6758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:8">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>501</v>
       </c>
@@ -6756,7 +6784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:8">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>504</v>
       </c>
@@ -6782,7 +6810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:8">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>507</v>
       </c>
@@ -6808,7 +6836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:8">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>510</v>
       </c>
@@ -6834,7 +6862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:8">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>513</v>
       </c>
@@ -6860,7 +6888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:8">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>516</v>
       </c>
@@ -6886,7 +6914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:8">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>519</v>
       </c>
@@ -6912,7 +6940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:8">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>522</v>
       </c>
@@ -6938,7 +6966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:8">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>525</v>
       </c>
@@ -6964,7 +6992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:8">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>528</v>
       </c>
@@ -6990,7 +7018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:8">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>531</v>
       </c>
@@ -7016,7 +7044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:8">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>534</v>
       </c>
@@ -7042,7 +7070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:8">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>537</v>
       </c>
@@ -7068,7 +7096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:8">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>540</v>
       </c>
@@ -7094,7 +7122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:8">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>543</v>
       </c>
@@ -7120,7 +7148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:8">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>546</v>
       </c>
@@ -7146,7 +7174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:8">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>549</v>
       </c>
@@ -7172,7 +7200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:8">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>552</v>
       </c>
@@ -7198,7 +7226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:8">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>555</v>
       </c>
@@ -7224,7 +7252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:8">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>558</v>
       </c>
@@ -7250,7 +7278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:8">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>561</v>
       </c>
@@ -7276,7 +7304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:8">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>564</v>
       </c>
@@ -7302,7 +7330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:8">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>567</v>
       </c>
@@ -7328,7 +7356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:8">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>570</v>
       </c>
@@ -7354,7 +7382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:8">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>573</v>
       </c>
@@ -7380,7 +7408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:8">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>576</v>
       </c>
@@ -7406,7 +7434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:8">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>579</v>
       </c>
@@ -7432,7 +7460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:8">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>582</v>
       </c>
@@ -7458,7 +7486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:8">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>584</v>
       </c>
@@ -7484,7 +7512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:8">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>587</v>
       </c>
@@ -7510,7 +7538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:8">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>590</v>
       </c>
@@ -7536,7 +7564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:8">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>593</v>
       </c>
@@ -7562,7 +7590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:8">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>596</v>
       </c>
@@ -7588,7 +7616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:8">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>599</v>
       </c>
@@ -7614,7 +7642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:8">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>602</v>
       </c>
@@ -7640,7 +7668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:8">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>605</v>
       </c>
@@ -7666,7 +7694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:8">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>608</v>
       </c>
@@ -7692,7 +7720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:8">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>611</v>
       </c>
@@ -7718,7 +7746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:8">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>614</v>
       </c>
@@ -7754,20 +7782,20 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A3" sqref="A3:A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="4" width="34.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" customWidth="1"/>
+    <col min="4" max="4" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>617</v>
       </c>
@@ -7793,7 +7821,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.95">
+    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>620</v>
       </c>
@@ -7815,7 +7843,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="17.100000000000001">
+    <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>622</v>
       </c>
@@ -7835,7 +7863,7 @@
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:8" ht="17.100000000000001">
+    <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>624</v>
       </c>
@@ -7855,7 +7883,7 @@
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:8" ht="17.100000000000001">
+    <row r="5" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>625</v>
       </c>
@@ -7875,7 +7903,7 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:8" ht="51">
+    <row r="6" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>626</v>
       </c>
@@ -7895,7 +7923,7 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:8" ht="51">
+    <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>629</v>
       </c>
@@ -7915,7 +7943,7 @@
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="1:8" ht="51">
+    <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>630</v>
       </c>
@@ -7935,9 +7963,9 @@
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:8" ht="33.950000000000003">
+    <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>631</v>
+        <v>669</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>627</v>
@@ -7955,18 +7983,18 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:8" ht="33.950000000000003">
+    <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
+        <v>631</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>632</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="C10" s="3" t="s">
         <v>633</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>634</v>
-      </c>
       <c r="D10" s="3" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="E10" s="3">
         <v>300</v>
@@ -7975,12 +8003,12 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:8" ht="33.950000000000003">
+    <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>623</v>
@@ -7997,9 +8025,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="17.100000000000001">
+    <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>14</v>
@@ -8019,15 +8047,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="17.100000000000001">
+    <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
+        <v>636</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>637</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>638</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>639</v>
       </c>
       <c r="D13" s="3">
         <v>2.7027026999999999E-2</v>
@@ -8039,12 +8067,12 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:8" ht="33.950000000000003">
+    <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>623</v>
@@ -8061,12 +8089,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="33.950000000000003">
+    <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>623</v>
@@ -8083,18 +8111,18 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="17.100000000000001">
+    <row r="16" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="E16" s="3">
         <v>0</v>
@@ -8103,18 +8131,18 @@
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="1:5" ht="33.950000000000003">
+    <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
+        <v>642</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>643</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>644</v>
-      </c>
       <c r="C17" s="3" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="E17" s="3">
         <v>0</v>
@@ -8130,17 +8158,17 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>617</v>
       </c>
@@ -8163,18 +8191,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.95">
+    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>644</v>
+      </c>
+      <c r="B2" t="s">
         <v>645</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>646</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>647</v>
-      </c>
-      <c r="D2" t="s">
-        <v>648</v>
       </c>
       <c r="E2">
         <v>-20</v>
@@ -8183,12 +8211,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.95">
+    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="B3" t="s">
         <v>649</v>
-      </c>
-      <c r="B3" t="s">
-        <v>650</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -8197,35 +8225,35 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>650</v>
+      </c>
+      <c r="B4" t="s">
         <v>651</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>652</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>653</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>654</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>655</v>
       </c>
-      <c r="G4" t="s">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>656</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>657</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>658</v>
-      </c>
-      <c r="C5" t="s">
-        <v>659</v>
       </c>
       <c r="D5">
         <v>0.58899999999999997</v>
@@ -8243,15 +8271,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3414DD4-9A5D-DA4B-8243-98C74F16DBC8}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="1" max="1" width="26.83203125" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>617</v>
       </c>
@@ -8259,68 +8289,1935 @@
         <v>618</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.95">
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="B2" t="s">
         <v>660</v>
       </c>
+    </row>
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="B3" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>662</v>
+      </c>
+      <c r="B4" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="B5" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>664</v>
+      </c>
+      <c r="B6" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>665</v>
+      </c>
+      <c r="B7" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>666</v>
+      </c>
+      <c r="B8" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>667</v>
+      </c>
+      <c r="B9" t="s">
+        <v>660</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F0C1640-7785-9A40-A4A4-5C1F9E6B7D30}">
+  <dimension ref="A1:B231"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="51.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
       <c r="B2" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>94</v>
+      </c>
+      <c r="B28" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>97</v>
+      </c>
+      <c r="B29" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>100</v>
+      </c>
+      <c r="B30" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>103</v>
+      </c>
+      <c r="B31" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>106</v>
+      </c>
+      <c r="B32" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>109</v>
+      </c>
+      <c r="B33" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>112</v>
+      </c>
+      <c r="B34" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>115</v>
+      </c>
+      <c r="B35" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>118</v>
+      </c>
+      <c r="B36" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>121</v>
+      </c>
+      <c r="B37" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>124</v>
+      </c>
+      <c r="B38" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>127</v>
+      </c>
+      <c r="B39" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>130</v>
+      </c>
+      <c r="B40" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>133</v>
+      </c>
+      <c r="B41" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>136</v>
+      </c>
+      <c r="B42" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>139</v>
+      </c>
+      <c r="B43" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>142</v>
+      </c>
+      <c r="B44" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>145</v>
+      </c>
+      <c r="B45" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>148</v>
+      </c>
+      <c r="B46" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>151</v>
+      </c>
+      <c r="B47" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>154</v>
+      </c>
+      <c r="B48" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>157</v>
+      </c>
+      <c r="B49" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>160</v>
+      </c>
+      <c r="B50" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>163</v>
+      </c>
+      <c r="B51" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>166</v>
+      </c>
+      <c r="B52" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>169</v>
+      </c>
+      <c r="B53" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>172</v>
+      </c>
+      <c r="B54" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>175</v>
+      </c>
+      <c r="B55" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>178</v>
+      </c>
+      <c r="B56" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>181</v>
+      </c>
+      <c r="B57" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>184</v>
+      </c>
+      <c r="B58" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>187</v>
+      </c>
+      <c r="B59" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>190</v>
+      </c>
+      <c r="B60" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>193</v>
+      </c>
+      <c r="B61" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>196</v>
+      </c>
+      <c r="B62" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>199</v>
+      </c>
+      <c r="B63" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>202</v>
+      </c>
+      <c r="B64" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>205</v>
+      </c>
+      <c r="B65" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>208</v>
+      </c>
+      <c r="B66" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>211</v>
+      </c>
+      <c r="B67" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>214</v>
+      </c>
+      <c r="B68" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>217</v>
+      </c>
+      <c r="B69" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>220</v>
+      </c>
+      <c r="B70" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>223</v>
+      </c>
+      <c r="B71" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>226</v>
+      </c>
+      <c r="B72" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>229</v>
+      </c>
+      <c r="B73" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>232</v>
+      </c>
+      <c r="B74" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>235</v>
+      </c>
+      <c r="B75" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>238</v>
+      </c>
+      <c r="B76" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>241</v>
+      </c>
+      <c r="B77" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>244</v>
+      </c>
+      <c r="B78" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>247</v>
+      </c>
+      <c r="B79" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>250</v>
+      </c>
+      <c r="B80" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>253</v>
+      </c>
+      <c r="B81" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>256</v>
+      </c>
+      <c r="B82" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>259</v>
+      </c>
+      <c r="B83" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>262</v>
+      </c>
+      <c r="B84" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>265</v>
+      </c>
+      <c r="B85" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>268</v>
+      </c>
+      <c r="B86" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>271</v>
+      </c>
+      <c r="B87" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>274</v>
+      </c>
+      <c r="B88" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>277</v>
+      </c>
+      <c r="B89" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>280</v>
+      </c>
+      <c r="B90" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>282</v>
+      </c>
+      <c r="B91" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>285</v>
+      </c>
+      <c r="B92" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>288</v>
+      </c>
+      <c r="B93" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>291</v>
+      </c>
+      <c r="B94" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>294</v>
+      </c>
+      <c r="B95" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>297</v>
+      </c>
+      <c r="B96" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>300</v>
+      </c>
+      <c r="B97" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>303</v>
+      </c>
+      <c r="B98" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>306</v>
+      </c>
+      <c r="B99" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>309</v>
+      </c>
+      <c r="B100" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>312</v>
+      </c>
+      <c r="B101" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>315</v>
+      </c>
+      <c r="B102" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>318</v>
+      </c>
+      <c r="B103" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>285</v>
+      </c>
+      <c r="B104" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>323</v>
+      </c>
+      <c r="B105" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>326</v>
+      </c>
+      <c r="B106" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>329</v>
+      </c>
+      <c r="B107" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>332</v>
+      </c>
+      <c r="B108" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>335</v>
+      </c>
+      <c r="B109" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>338</v>
+      </c>
+      <c r="B110" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>341</v>
+      </c>
+      <c r="B111" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>343</v>
+      </c>
+      <c r="B112" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>346</v>
+      </c>
+      <c r="B113" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>349</v>
+      </c>
+      <c r="B114" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>352</v>
+      </c>
+      <c r="B115" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>355</v>
+      </c>
+      <c r="B116" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>358</v>
+      </c>
+      <c r="B117" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>361</v>
+      </c>
+      <c r="B118" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>364</v>
+      </c>
+      <c r="B119" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>367</v>
+      </c>
+      <c r="B120" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>370</v>
+      </c>
+      <c r="B121" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>373</v>
+      </c>
+      <c r="B122" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>376</v>
+      </c>
+      <c r="B123" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>379</v>
+      </c>
+      <c r="B124" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>382</v>
+      </c>
+      <c r="B125" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>385</v>
+      </c>
+      <c r="B126" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>388</v>
+      </c>
+      <c r="B127" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>391</v>
+      </c>
+      <c r="B128" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>394</v>
+      </c>
+      <c r="B129" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>397</v>
+      </c>
+      <c r="B130" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>400</v>
+      </c>
+      <c r="B131" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>403</v>
+      </c>
+      <c r="B132" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>406</v>
+      </c>
+      <c r="B133" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>409</v>
+      </c>
+      <c r="B134" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>412</v>
+      </c>
+      <c r="B135" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>415</v>
+      </c>
+      <c r="B136" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>418</v>
+      </c>
+      <c r="B137" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>421</v>
+      </c>
+      <c r="B138" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>424</v>
+      </c>
+      <c r="B139" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>427</v>
+      </c>
+      <c r="B140" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>430</v>
+      </c>
+      <c r="B141" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>433</v>
+      </c>
+      <c r="B142" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>436</v>
+      </c>
+      <c r="B143" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>439</v>
+      </c>
+      <c r="B144" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>442</v>
+      </c>
+      <c r="B145" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>445</v>
+      </c>
+      <c r="B146" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>448</v>
+      </c>
+      <c r="B147" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>451</v>
+      </c>
+      <c r="B148" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>454</v>
+      </c>
+      <c r="B149" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>457</v>
+      </c>
+      <c r="B150" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>460</v>
+      </c>
+      <c r="B151" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>463</v>
+      </c>
+      <c r="B152" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>466</v>
+      </c>
+      <c r="B153" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>469</v>
+      </c>
+      <c r="B154" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>472</v>
+      </c>
+      <c r="B155" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>475</v>
+      </c>
+      <c r="B156" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>478</v>
+      </c>
+      <c r="B157" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>481</v>
+      </c>
+      <c r="B158" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>484</v>
+      </c>
+      <c r="B159" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>487</v>
+      </c>
+      <c r="B160" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>490</v>
+      </c>
+      <c r="B161" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>493</v>
+      </c>
+      <c r="B162" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>496</v>
+      </c>
+      <c r="B163" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>499</v>
+      </c>
+      <c r="B164" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>502</v>
+      </c>
+      <c r="B165" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>505</v>
+      </c>
+      <c r="B166" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>508</v>
+      </c>
+      <c r="B167" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>511</v>
+      </c>
+      <c r="B168" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>514</v>
+      </c>
+      <c r="B169" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>517</v>
+      </c>
+      <c r="B170" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>520</v>
+      </c>
+      <c r="B171" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>523</v>
+      </c>
+      <c r="B172" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>526</v>
+      </c>
+      <c r="B173" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>529</v>
+      </c>
+      <c r="B174" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>532</v>
+      </c>
+      <c r="B175" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>535</v>
+      </c>
+      <c r="B176" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>538</v>
+      </c>
+      <c r="B177" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>541</v>
+      </c>
+      <c r="B178" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>544</v>
+      </c>
+      <c r="B179" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>547</v>
+      </c>
+      <c r="B180" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>550</v>
+      </c>
+      <c r="B181" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>553</v>
+      </c>
+      <c r="B182" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>556</v>
+      </c>
+      <c r="B183" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>559</v>
+      </c>
+      <c r="B184" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
+        <v>562</v>
+      </c>
+      <c r="B185" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>565</v>
+      </c>
+      <c r="B186" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>568</v>
+      </c>
+      <c r="B187" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>571</v>
+      </c>
+      <c r="B188" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>574</v>
+      </c>
+      <c r="B189" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>577</v>
+      </c>
+      <c r="B190" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>580</v>
+      </c>
+      <c r="B191" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>583</v>
+      </c>
+      <c r="B192" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>585</v>
+      </c>
+      <c r="B193" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>588</v>
+      </c>
+      <c r="B194" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>591</v>
+      </c>
+      <c r="B195" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>594</v>
+      </c>
+      <c r="B196" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
+        <v>597</v>
+      </c>
+      <c r="B197" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
+        <v>600</v>
+      </c>
+      <c r="B198" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
+        <v>603</v>
+      </c>
+      <c r="B199" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>606</v>
+      </c>
+      <c r="B200" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
+        <v>609</v>
+      </c>
+      <c r="B201" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
+        <v>612</v>
+      </c>
+      <c r="B202" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>615</v>
+      </c>
+      <c r="B203" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>620</v>
+      </c>
+      <c r="B204" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A205" s="7" t="s">
+        <v>622</v>
+      </c>
+      <c r="B205" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A206" s="7" t="s">
+        <v>624</v>
+      </c>
+      <c r="B206" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A207" s="7" t="s">
+        <v>625</v>
+      </c>
+      <c r="B207" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A208" s="7" t="s">
+        <v>626</v>
+      </c>
+      <c r="B208" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A209" s="7" t="s">
+        <v>629</v>
+      </c>
+      <c r="B209" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A210" s="7" t="s">
+        <v>630</v>
+      </c>
+      <c r="B210" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A211" s="7" t="s">
+        <v>669</v>
+      </c>
+      <c r="B211" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A212" s="7" t="s">
+        <v>631</v>
+      </c>
+      <c r="B212" s="7" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A213" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="B213" s="7" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A214" s="7" t="s">
+        <v>635</v>
+      </c>
+      <c r="B214" s="7" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A215" s="7" t="s">
+        <v>636</v>
+      </c>
+      <c r="B215" s="7" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A216" s="7" t="s">
+        <v>639</v>
+      </c>
+      <c r="B216" s="7" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A217" s="7" t="s">
+        <v>640</v>
+      </c>
+      <c r="B217" s="7" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A218" s="7" t="s">
+        <v>641</v>
+      </c>
+      <c r="B218" s="7" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A219" s="7" t="s">
+        <v>642</v>
+      </c>
+      <c r="B219" s="7" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A220" s="2" t="s">
+        <v>644</v>
+      </c>
+      <c r="B220" s="2" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A221" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="B221" s="2" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A222" t="s">
+        <v>650</v>
+      </c>
+      <c r="B222" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A223" t="s">
+        <v>656</v>
+      </c>
+      <c r="B223" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A224" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="B224" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A225" s="2" t="s">
         <v>661</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.95">
-      <c r="A3" s="2" t="s">
+      <c r="B225" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A226" s="2" t="s">
         <v>662</v>
       </c>
-      <c r="B3" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="32.1">
-      <c r="A4" s="2" t="s">
+      <c r="B226" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A227" s="2" t="s">
         <v>663</v>
       </c>
-      <c r="B4" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.95">
-      <c r="A5" s="2" t="s">
+      <c r="B227" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A228" s="2" t="s">
         <v>664</v>
       </c>
-      <c r="B5" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="63.95">
-      <c r="A6" s="2" t="s">
+      <c r="B228" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A229" s="2" t="s">
         <v>665</v>
       </c>
-      <c r="B6" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.95">
-      <c r="A7" s="2" t="s">
+      <c r="B229" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A230" s="2" t="s">
         <v>666</v>
       </c>
-      <c r="B7" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15.95">
-      <c r="A8" s="2" t="s">
+      <c r="B230" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A231" s="2" t="s">
         <v>667</v>
       </c>
-      <c r="B8" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15.95">
-      <c r="A9" s="2" t="s">
-        <v>668</v>
-      </c>
-      <c r="B9" t="s">
-        <v>661</v>
+      <c r="B231" t="s">
+        <v>673</v>
       </c>
     </row>
   </sheetData>
@@ -8329,22 +10226,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8cbc129c-3b7a-4ec6-bc99-044e863a9e9b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="41fbb2c2-4ead-45c8-9603-90a6437e6117" xsi:nil="true"/>
-    <gc7d5424db48485e84a88e64a4f291ed xmlns="8cbc129c-3b7a-4ec6-bc99-044e863a9e9b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </gc7d5424db48485e84a88e64a4f291ed>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009A6E36D7387735418D866E0DCE87A730" ma:contentTypeVersion="21" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="fcb2cb28cadb0ba0f0f8b4739691dd15">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8cbc129c-3b7a-4ec6-bc99-044e863a9e9b" xmlns:ns3="41fbb2c2-4ead-45c8-9603-90a6437e6117" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="10d101666b3ec76555eb3f6a5bab6d17" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009A6E36D7387735418D866E0DCE87A730" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fb8f9a572e79264b8dc3d6c17170b7e3">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8cbc129c-3b7a-4ec6-bc99-044e863a9e9b" xmlns:ns3="41fbb2c2-4ead-45c8-9603-90a6437e6117" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0c70e2f6acecb963727c057e32a00f5b" ns2:_="" ns3:_="">
     <xsd:import namespace="8cbc129c-3b7a-4ec6-bc99-044e863a9e9b"/>
     <xsd:import namespace="41fbb2c2-4ead-45c8-9603-90a6437e6117"/>
     <xsd:element name="properties">
@@ -8440,7 +10332,7 @@
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="22" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Balises d’images" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="0221fbda-75be-4c33-b0c8-319ad1a56315" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="22" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="0221fbda-75be-4c33-b0c8-319ad1a56315" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
@@ -8468,7 +10360,7 @@
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="41fbb2c2-4ead-45c8-9603-90a6437e6117" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="17" nillable="true" ma:displayName="Partagé avec" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="17" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -8487,7 +10379,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="18" nillable="true" ma:displayName="Partagé avec détails" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="18" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -8515,8 +10407,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Type de contenu"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titre"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -8606,22 +10498,59 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8cbc129c-3b7a-4ec6-bc99-044e863a9e9b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="41fbb2c2-4ead-45c8-9603-90a6437e6117" xsi:nil="true"/>
+    <gc7d5424db48485e84a88e64a4f291ed xmlns="8cbc129c-3b7a-4ec6-bc99-044e863a9e9b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </gc7d5424db48485e84a88e64a4f291ed>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0AB6737F-05DC-4189-932B-A793C8F33C83}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF33073B-FF4D-49A0-AC16-CF9FD1E6B2A8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38FC957A-A433-4DD8-9E1B-673B48D75BB4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7380BC32-8A77-4197-AF98-9A6ECAAB3A34}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8cbc129c-3b7a-4ec6-bc99-044e863a9e9b"/>
+    <ds:schemaRef ds:uri="41fbb2c2-4ead-45c8-9603-90a6437e6117"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF33073B-FF4D-49A0-AC16-CF9FD1E6B2A8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0AB6737F-05DC-4189-932B-A793C8F33C83}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8cbc129c-3b7a-4ec6-bc99-044e863a9e9b"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="41fbb2c2-4ead-45c8-9603-90a6437e6117"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>